<commit_message>
modified data for getTrainsStatus test
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/getTrainStatus.xlsx
+++ b/src/test/resources/datasheets/getTrainStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bajwauto\Projects\MultiAppPOM\multiApp\src\test\resources\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA5DCBA-C5F0-4567-B72C-A180411A7BCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5492D93B-364D-448A-911A-95C2E97BE970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>today</t>
   </si>
   <si>
-    <t>Swarna Shatabdi</t>
-  </si>
-  <si>
     <t>UMB</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>departureDay</t>
+  </si>
+  <si>
+    <t>Uhl Janstb Spl</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +414,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -425,7 +425,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
@@ -436,10 +436,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>

</xml_diff>